<commit_message>
Removed a irrelevant entropy case
</commit_message>
<xml_diff>
--- a/Technical Debt Backlog.xlsx
+++ b/Technical Debt Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suwic\Downloads\Repository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4DCBAB2-E432-4DB0-ACE5-126E7E9D84A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63CE8A0E-6911-4B37-8646-62262F808D5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-315" yWindow="2115" windowWidth="24225" windowHeight="13590" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="2145" windowWidth="12240" windowHeight="13590" firstSheet="9" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="File Properties" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="185">
   <si>
     <t>Filename</t>
   </si>
@@ -286,12 +286,6 @@
   </si>
   <si>
     <t>Interest-based Ranked Pr</t>
-  </si>
-  <si>
-    <t>Coin</t>
-  </si>
-  <si>
-    <t>Coin Pr</t>
   </si>
   <si>
     <t>Schmid's (Original)</t>
@@ -1324,7 +1318,7 @@
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -1345,8 +1339,8 @@
   </sheetPr>
   <dimension ref="A1:AK26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AG10" sqref="AG10:AK14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1523,91 +1517,36 @@
       </c>
     </row>
     <row r="10" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AG10" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH10" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AI10" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AJ10" s="1" t="s">
-        <v>83</v>
-      </c>
+      <c r="AG10" s="1"/>
+      <c r="AH10" s="1"/>
+      <c r="AI10" s="1"/>
+      <c r="AJ10" s="1"/>
     </row>
     <row r="11" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="AG11" s="1">
-        <v>1</v>
-      </c>
-      <c r="AH11" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="AI11" s="1">
-        <v>1</v>
-      </c>
-      <c r="AJ11" s="1">
-        <f t="shared" ref="AJ11:AJ13" si="0">AI11/SUM($AI$11:$AI$13)</f>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="AK11" s="4">
-        <f t="shared" ref="AK11:AK13" si="1">-1*(AJ11*LOG(AJ11,2))</f>
-        <v>0.43082708345352599</v>
-      </c>
+      <c r="AG11" s="1"/>
+      <c r="AH11" s="1"/>
+      <c r="AI11" s="1"/>
+      <c r="AJ11" s="1"/>
+      <c r="AK11" s="4"/>
     </row>
     <row r="12" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="AG12" s="1">
-        <v>1</v>
-      </c>
-      <c r="AH12" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="AI12" s="1">
-        <v>2</v>
-      </c>
-      <c r="AJ12" s="1">
-        <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="AK12" s="4">
-        <f t="shared" si="1"/>
-        <v>0.52832083357371873</v>
-      </c>
+      <c r="AG12" s="1"/>
+      <c r="AH12" s="1"/>
+      <c r="AI12" s="1"/>
+      <c r="AJ12" s="1"/>
+      <c r="AK12" s="4"/>
     </row>
     <row r="13" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="AG13" s="4">
-        <f t="shared" ref="AG13:AH13" si="2">SUM(AG11:AG12)</f>
-        <v>2</v>
-      </c>
-      <c r="AH13" s="4">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="AI13" s="1">
-        <v>3</v>
-      </c>
-      <c r="AJ13" s="1">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="AK13" s="4">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
+      <c r="AG13" s="4"/>
+      <c r="AH13" s="4"/>
+      <c r="AI13" s="1"/>
+      <c r="AJ13" s="1"/>
+      <c r="AK13" s="4"/>
     </row>
     <row r="14" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="AI14" s="4">
-        <f t="shared" ref="AI14:AJ14" si="3">SUM(AI11:AI12)</f>
-        <v>3</v>
-      </c>
-      <c r="AJ14" s="4">
-        <f t="shared" si="3"/>
-        <v>0.5</v>
-      </c>
-      <c r="AK14" s="4">
-        <f>SUM(AK11:AK13)</f>
-        <v>1.4591479170272448</v>
-      </c>
+      <c r="AI14" s="4"/>
+      <c r="AJ14" s="4"/>
+      <c r="AK14" s="4"/>
     </row>
     <row r="15" spans="1:37" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="16" spans="1:37" ht="12.75" x14ac:dyDescent="0.2"/>
@@ -1649,7 +1588,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1727,7 +1666,7 @@
         <v>20</v>
       </c>
       <c r="B1" s="55" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C1" s="55" t="s">
         <v>26</v>
@@ -1739,13 +1678,13 @@
       <c r="F1" s="55"/>
       <c r="G1" s="55"/>
       <c r="H1" s="55" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" s="56" t="s">
         <v>102</v>
-      </c>
-      <c r="I1" s="55" t="s">
-        <v>103</v>
-      </c>
-      <c r="J1" s="56" t="s">
-        <v>104</v>
       </c>
       <c r="K1" s="55"/>
       <c r="L1" s="55"/>
@@ -1766,10 +1705,10 @@
         <v>8</v>
       </c>
       <c r="F2" s="36" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G2" s="36" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H2" s="55"/>
       <c r="I2" s="55"/>
@@ -1780,7 +1719,7 @@
         <v>8</v>
       </c>
       <c r="L2" s="36" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="M2" s="36" t="s">
         <v>26</v>
@@ -1798,7 +1737,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D3" s="36">
         <v>0.1</v>
@@ -1817,7 +1756,7 @@
         <v>180</v>
       </c>
       <c r="I3" s="36" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J3" s="36">
         <v>0.5</v>
@@ -1829,7 +1768,7 @@
         <v>0.6</v>
       </c>
       <c r="M3" s="36" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:36" ht="15" x14ac:dyDescent="0.25">
@@ -1838,7 +1777,7 @@
       </c>
       <c r="B4" s="38"/>
       <c r="C4" s="36" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D4" s="36">
         <v>0.3</v>
@@ -1854,10 +1793,10 @@
         <v>8.2753657951547113E-2</v>
       </c>
       <c r="H4" s="36" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I4" s="36" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J4" s="36">
         <v>0.35</v>
@@ -1869,7 +1808,7 @@
         <v>0.4</v>
       </c>
       <c r="M4" s="36" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:36" ht="15" x14ac:dyDescent="0.25">
@@ -1880,7 +1819,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D5" s="36">
         <v>0.1</v>
@@ -1899,7 +1838,7 @@
         <v>30</v>
       </c>
       <c r="I5" s="36" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J5" s="36">
         <v>0.35</v>
@@ -1911,7 +1850,7 @@
         <v>0.4</v>
       </c>
       <c r="M5" s="36" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:36" ht="15" x14ac:dyDescent="0.25">
@@ -1920,7 +1859,7 @@
       </c>
       <c r="B6" s="38"/>
       <c r="C6" s="36" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D6" s="36">
         <v>0.4</v>
@@ -1939,7 +1878,7 @@
         <v>260</v>
       </c>
       <c r="I6" s="36" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J6" s="36">
         <v>0.6</v>
@@ -1951,7 +1890,7 @@
         <v>0.7</v>
       </c>
       <c r="M6" s="36" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:36" ht="15" x14ac:dyDescent="0.25">
@@ -1960,7 +1899,7 @@
       </c>
       <c r="B7" s="38"/>
       <c r="C7" s="36" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D7" s="36">
         <v>0.4</v>
@@ -1976,10 +1915,10 @@
         <v>0.1067402254737347</v>
       </c>
       <c r="H7" s="36" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I7" s="36" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J7" s="36">
         <v>0.1</v>
@@ -1991,7 +1930,7 @@
         <v>0.12</v>
       </c>
       <c r="M7" s="36" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:36" ht="15" x14ac:dyDescent="0.25">
@@ -2002,7 +1941,7 @@
         <v>15</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D8" s="36">
         <v>0.2</v>
@@ -2021,7 +1960,7 @@
         <v>10</v>
       </c>
       <c r="I8" s="36" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J8" s="36">
         <v>0.1</v>
@@ -2033,7 +1972,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="M8" s="36" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:36" ht="15" x14ac:dyDescent="0.25">
@@ -2042,7 +1981,7 @@
       </c>
       <c r="B9" s="38"/>
       <c r="C9" s="36" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D9" s="36">
         <v>0.5</v>
@@ -2061,7 +2000,7 @@
         <v>20</v>
       </c>
       <c r="I9" s="36" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J9" s="36">
         <v>0.7</v>
@@ -2073,7 +2012,7 @@
         <v>0.76</v>
       </c>
       <c r="M9" s="36" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:36" ht="15" x14ac:dyDescent="0.25">
@@ -2084,7 +2023,7 @@
         <v>17</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D10" s="36">
         <v>0.05</v>
@@ -2103,7 +2042,7 @@
         <v>90</v>
       </c>
       <c r="I10" s="36" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J10" s="36">
         <v>0.2</v>
@@ -2115,7 +2054,7 @@
         <v>0.37</v>
       </c>
       <c r="M10" s="36" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:36" ht="15" x14ac:dyDescent="0.25">
@@ -2126,7 +2065,7 @@
         <v>18</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D11" s="36">
         <v>0.1</v>
@@ -2145,7 +2084,7 @@
         <v>4</v>
       </c>
       <c r="I11" s="36" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J11" s="36">
         <v>0.7</v>
@@ -2157,7 +2096,7 @@
         <v>0.75</v>
       </c>
       <c r="M11" s="36" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:36" ht="15" x14ac:dyDescent="0.25">
@@ -2166,7 +2105,7 @@
       </c>
       <c r="B12" s="38"/>
       <c r="C12" s="36" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D12" s="36">
         <v>0.4</v>
@@ -2185,7 +2124,7 @@
         <v>40</v>
       </c>
       <c r="I12" s="36" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J12" s="36">
         <v>0.6</v>
@@ -2197,7 +2136,7 @@
         <v>0.65</v>
       </c>
       <c r="M12" s="36" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:36" ht="15" x14ac:dyDescent="0.25">
@@ -2206,7 +2145,7 @@
       </c>
       <c r="B13" s="38"/>
       <c r="C13" s="36" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D13" s="36">
         <v>0.2</v>
@@ -2225,7 +2164,7 @@
         <v>10</v>
       </c>
       <c r="I13" s="36" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J13" s="36">
         <v>0.4</v>
@@ -2237,7 +2176,7 @@
         <v>0.47</v>
       </c>
       <c r="M13" s="36" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:36" ht="15" x14ac:dyDescent="0.25">
@@ -2248,7 +2187,7 @@
         <v>19</v>
       </c>
       <c r="C14" s="36" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D14" s="36">
         <v>0.15</v>
@@ -2267,7 +2206,7 @@
         <v>10</v>
       </c>
       <c r="I14" s="36" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J14" s="36">
         <v>0.1</v>
@@ -2279,7 +2218,7 @@
         <v>0.13</v>
       </c>
       <c r="M14" s="36" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:36" ht="15" x14ac:dyDescent="0.25">
@@ -2288,7 +2227,7 @@
       </c>
       <c r="B15" s="38"/>
       <c r="C15" s="36" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D15" s="36">
         <v>0.2</v>
@@ -2307,7 +2246,7 @@
         <v>40</v>
       </c>
       <c r="I15" s="36" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J15" s="36">
         <v>0.25</v>
@@ -2319,7 +2258,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="M15" s="36" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:36" ht="15" x14ac:dyDescent="0.25">
@@ -2328,7 +2267,7 @@
       </c>
       <c r="B16" s="38"/>
       <c r="C16" s="36" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D16" s="36">
         <v>0.25</v>
@@ -2344,10 +2283,10 @@
         <v>6.6202926361237702E-2</v>
       </c>
       <c r="H16" s="36" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I16" s="36" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J16" s="36">
         <v>0.1</v>
@@ -2359,7 +2298,7 @@
         <v>0.12</v>
       </c>
       <c r="M16" s="36" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2385,7 +2324,7 @@
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="12.75" x14ac:dyDescent="0.2"/>
@@ -2439,30 +2378,30 @@
   <sheetData>
     <row r="1" spans="1:14" s="10" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="57" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>41</v>
@@ -2480,7 +2419,7 @@
         <v>0.22800000000000001</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J2" s="16"/>
       <c r="K2" s="16"/>
@@ -2491,7 +2430,7 @@
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="57"/>
       <c r="B3" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>49</v>
@@ -2518,7 +2457,7 @@
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="57"/>
       <c r="B4" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>50</v>
@@ -2536,7 +2475,7 @@
         <v>0.48099999999999998</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J4" s="19"/>
       <c r="K4" s="19"/>
@@ -2556,7 +2495,7 @@
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="57"/>
       <c r="B5" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>55</v>
@@ -2574,7 +2513,7 @@
         <v>0.32400000000000001</v>
       </c>
       <c r="I5" s="21" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="J5" s="19"/>
       <c r="K5" s="19"/>
@@ -2594,7 +2533,7 @@
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="57"/>
       <c r="B6" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>43</v>
@@ -2612,7 +2551,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="I6" s="21" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J6" s="19"/>
       <c r="K6" s="19"/>
@@ -2632,7 +2571,7 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="57"/>
       <c r="B7" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>56</v>
@@ -2650,7 +2589,7 @@
         <v>0.17399999999999999</v>
       </c>
       <c r="I7" s="21" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J7" s="19"/>
       <c r="K7" s="19"/>
@@ -2670,7 +2609,7 @@
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="57"/>
       <c r="B8" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>51</v>
@@ -2688,7 +2627,7 @@
         <v>0.44800000000000001</v>
       </c>
       <c r="I8" s="21" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J8" s="19"/>
       <c r="K8" s="19"/>
@@ -2708,7 +2647,7 @@
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="57"/>
       <c r="B9" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>44</v>
@@ -2726,7 +2665,7 @@
         <v>0.26800000000000002</v>
       </c>
       <c r="I9" s="21" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J9" s="19"/>
       <c r="K9" s="19"/>
@@ -2746,7 +2685,7 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="57"/>
       <c r="B10" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>45</v>
@@ -2764,7 +2703,7 @@
         <v>0.20300000000000001</v>
       </c>
       <c r="I10" s="21" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J10" s="19"/>
       <c r="K10" s="19"/>
@@ -2784,7 +2723,7 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="57"/>
       <c r="B11" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>52</v>
@@ -2802,7 +2741,7 @@
         <v>0.224</v>
       </c>
       <c r="I11" s="21" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J11" s="19"/>
       <c r="K11" s="19"/>
@@ -2821,10 +2760,10 @@
     </row>
     <row r="12" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="57" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>48</v>
@@ -2842,7 +2781,7 @@
         <v>0.34499999999999997</v>
       </c>
       <c r="I12" s="21" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="J12" s="19"/>
       <c r="K12" s="19"/>
@@ -2862,7 +2801,7 @@
     <row r="13" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="57"/>
       <c r="B13" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>54</v>
@@ -2880,7 +2819,7 @@
         <v>0.44500000000000001</v>
       </c>
       <c r="I13" s="21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J13" s="19"/>
       <c r="K13" s="19"/>
@@ -2900,7 +2839,7 @@
     <row r="14" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="57"/>
       <c r="B14" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>42</v>
@@ -2918,7 +2857,7 @@
         <v>0.54100000000000004</v>
       </c>
       <c r="I14" s="21" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J14" s="22"/>
       <c r="K14" s="22"/>
@@ -2938,7 +2877,7 @@
     <row r="15" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="57"/>
       <c r="B15" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>46</v>
@@ -2956,7 +2895,7 @@
         <v>0.27600000000000002</v>
       </c>
       <c r="I15" s="21" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J15" s="22"/>
       <c r="K15" s="22"/>
@@ -2989,10 +2928,10 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I17" s="24" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J17" s="19"/>
       <c r="K17" s="19"/>
@@ -3011,7 +2950,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="I18" s="24" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="J18" s="19"/>
       <c r="K18" s="19"/>
@@ -3030,7 +2969,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="I19" s="24" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J19" s="19"/>
       <c r="K19" s="19"/>
@@ -3049,7 +2988,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="I20" s="24" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="J20" s="19"/>
       <c r="K20" s="19"/>
@@ -3068,7 +3007,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="I21" s="24" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J21" s="19"/>
       <c r="K21" s="19"/>
@@ -3087,7 +3026,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="I22" s="24" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="J22" s="19"/>
       <c r="K22" s="19"/>
@@ -3114,7 +3053,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="I24" s="24" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J24" s="19"/>
       <c r="K24" s="19"/>
@@ -3133,7 +3072,7 @@
     </row>
     <row r="25" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="I25" s="27" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="J25" s="19"/>
       <c r="K25" s="28"/>
@@ -3149,7 +3088,7 @@
     </row>
     <row r="26" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="I26" s="31" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="J26" s="32"/>
       <c r="K26" s="32"/>
@@ -3207,7 +3146,7 @@
         <v>41</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3215,7 +3154,7 @@
         <v>48</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3223,7 +3162,7 @@
         <v>49</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3231,7 +3170,7 @@
         <v>50</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3239,7 +3178,7 @@
         <v>54</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3247,7 +3186,7 @@
         <v>55</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3255,7 +3194,7 @@
         <v>42</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3263,7 +3202,7 @@
         <v>43</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3271,7 +3210,7 @@
         <v>56</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3279,7 +3218,7 @@
         <v>51</v>
       </c>
       <c r="B12" s="36" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3287,7 +3226,7 @@
         <v>44</v>
       </c>
       <c r="B13" s="36" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3295,7 +3234,7 @@
         <v>45</v>
       </c>
       <c r="B14" s="36" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3303,7 +3242,7 @@
         <v>52</v>
       </c>
       <c r="B15" s="36" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3311,7 +3250,7 @@
         <v>46</v>
       </c>
       <c r="B16" s="36" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -3345,7 +3284,7 @@
         <v>20</v>
       </c>
       <c r="B1" s="56" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C1" s="55"/>
       <c r="D1" s="55"/>
@@ -3676,8 +3615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{005B68DA-C131-4B9B-9780-B444454CB2A4}">
   <dimension ref="A1:T18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3693,7 +3632,7 @@
         <v>20</v>
       </c>
       <c r="B1" s="56" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C1" s="55"/>
       <c r="D1" s="55"/>
@@ -3701,11 +3640,11 @@
       <c r="F1" s="55"/>
       <c r="G1" s="55"/>
       <c r="H1" s="55" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I1" s="55"/>
       <c r="J1" s="55" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K1" s="55"/>
       <c r="L1" s="55"/>
@@ -3718,7 +3657,7 @@
       <c r="Q1" s="55"/>
       <c r="R1" s="55"/>
       <c r="S1" s="56" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="T1" s="55"/>
     </row>
@@ -3737,43 +3676,43 @@
         <v>38</v>
       </c>
       <c r="F2" s="36" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G2" s="36" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H2" s="36" t="s">
         <v>32</v>
       </c>
       <c r="I2" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="J2" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="K2" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="J2" s="36" t="s">
+      <c r="L2" s="36" t="s">
         <v>113</v>
-      </c>
-      <c r="K2" s="36" t="s">
-        <v>114</v>
-      </c>
-      <c r="L2" s="36" t="s">
-        <v>115</v>
       </c>
       <c r="M2" s="36" t="s">
         <v>38</v>
       </c>
       <c r="N2" s="36" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="O2" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="P2" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q2" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="P2" s="36" t="s">
+      <c r="R2" s="36" t="s">
         <v>117</v>
-      </c>
-      <c r="Q2" s="36" t="s">
-        <v>118</v>
-      </c>
-      <c r="R2" s="36" t="s">
-        <v>119</v>
       </c>
       <c r="S2" s="36" t="s">
         <v>32</v>
@@ -4933,7 +4872,7 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -4953,8 +4892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98488B1C-4800-42D6-BF5F-3F0BAB4015AF}">
   <dimension ref="A1:AF37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6478,7 +6417,7 @@
       <c r="F18" s="38"/>
       <c r="G18" s="38"/>
       <c r="H18" s="36" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I18" s="40">
         <f>AVERAGE(I17,K17,M17)</f>
@@ -6509,13 +6448,13 @@
     <row r="20" spans="5:32" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="5:32" x14ac:dyDescent="0.2">
       <c r="H21" s="41" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="I21" s="42"/>
       <c r="J21" s="42"/>
       <c r="K21" s="42"/>
       <c r="L21" s="42" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="M21" s="42"/>
       <c r="N21" s="42"/>
@@ -6524,16 +6463,16 @@
     <row r="22" spans="5:32" x14ac:dyDescent="0.2">
       <c r="H22" s="44"/>
       <c r="I22" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="J22" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="K22" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="J22" s="45" t="s">
-        <v>91</v>
-      </c>
-      <c r="K22" s="45" t="s">
-        <v>92</v>
-      </c>
       <c r="L22" s="45" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="M22" s="45"/>
       <c r="N22" s="45"/>
@@ -6541,7 +6480,7 @@
     </row>
     <row r="23" spans="5:32" x14ac:dyDescent="0.2">
       <c r="H23" s="44" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I23" s="47">
         <f>($Z$17-I$17)/$Z$17</f>
@@ -6565,7 +6504,7 @@
     </row>
     <row r="24" spans="5:32" x14ac:dyDescent="0.2">
       <c r="H24" s="44" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I24" s="47">
         <f>($AC$17-I$17)/$AC$17</f>
@@ -6589,7 +6528,7 @@
     </row>
     <row r="25" spans="5:32" x14ac:dyDescent="0.2">
       <c r="H25" s="44" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I25" s="47">
         <f>($AF$17-I$17)/$AF$17</f>
@@ -6661,7 +6600,7 @@
     </row>
     <row r="28" spans="5:32" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="H28" s="48" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I28" s="51">
         <f>($T$17-I$17)/$T$17</f>
@@ -6961,7 +6900,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>